<commit_message>
Esop Pdf File save and Design
</commit_message>
<xml_diff>
--- a/src/assets/GrantExcelFormat.xlsx
+++ b/src/assets/GrantExcelFormat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cimply fema work\cimplyfema_app\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Date of Issue</t>
   </si>
@@ -62,12 +62,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Indian</t>
-  </si>
-  <si>
-    <t>Ashwani</t>
-  </si>
-  <si>
     <t>Viay</t>
   </si>
   <si>
@@ -78,6 +72,15 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>Resident</t>
+  </si>
+  <si>
+    <t>Non-Resident Indian</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +432,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -476,16 +479,16 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>500</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>500</v>
@@ -499,7 +502,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>44891</v>
@@ -511,16 +514,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <v>500</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3">
         <v>500</v>

</xml_diff>

<commit_message>
Form Esop save Changes PDF
</commit_message>
<xml_diff>
--- a/src/assets/GrantExcelFormat.xlsx
+++ b/src/assets/GrantExcelFormat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Date of Issue</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
   </si>
 </sst>
 </file>
@@ -127,8 +130,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +415,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,8 +472,8 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
-        <v>44891</v>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -504,8 +507,8 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
-        <v>44891</v>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C3">
         <v>100</v>

</xml_diff>